<commit_message>
Updated to funtional gears
</commit_message>
<xml_diff>
--- a/docs/Gears/Hip gears parameters.xlsx
+++ b/docs/Gears/Hip gears parameters.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7992"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="76">
   <si>
     <t>Fine Pitch Involute 20 deg</t>
   </si>
@@ -249,6 +250,9 @@
   </si>
   <si>
     <t>TERM</t>
+  </si>
+  <si>
+    <t>Coarse Pitch Involute 20 deg</t>
   </si>
 </sst>
 </file>
@@ -481,6 +485,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,10 +498,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,6 +819,1072 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.76969696969696966</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5">
+        <v>28.8636368847211</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.99352420357923</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.83103403183084</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1.68316162186012</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5">
+        <v>19.2424242424242</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="5">
+        <v>20.781818181818199</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5">
+        <v>17.318181818181799</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.76969696969696999</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.96212121212121204</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="5">
+        <v>18.081964066637799</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1.7318181818181799</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="5">
+        <v>2.4180743454904801</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5">
+        <v>0.23090909090909101</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1.2090371847152701</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="5">
+        <v>21.051904574067699</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5">
+        <v>3</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5">
+        <v>5.9501170921955202</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5">
+        <v>0</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="5">
+        <v>50</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="5">
+        <v>38.484848484848499</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="5">
+        <v>40.024242424242402</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="5">
+        <v>36.560606060606098</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0.76969696969696999</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.96212121212121204</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" s="5">
+        <v>36.163928133275597</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1.7318181818181799</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="5">
+        <v>2.4180743454904801</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5">
+        <v>0.23090909090909101</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1.2090371847152701</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="5">
+        <v>40.354460515376203</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5">
+        <v>6</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5">
+        <v>13.0363574826274</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4"/>
+      <c r="B64" s="5">
+        <v>0</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="4"/>
+      <c r="B65" s="5">
+        <v>0</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="4"/>
+      <c r="B66" s="5">
+        <v>0</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5">
+        <v>0</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5">
+        <v>0</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5">
+        <v>0</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="7"/>
+      <c r="B70" s="8">
+        <v>0</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="10"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="10"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="10"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="10"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="10"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="10"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="10"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="10"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="10"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="10"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="10"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="10"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="10"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A41:D41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="5.21875" customWidth="1"/>
     <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
@@ -949,12 +2019,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -1315,12 +2385,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
@@ -1669,196 +2739,196 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="10"/>
-      <c r="B70" s="11">
-        <v>0</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="12" t="s">
+      <c r="A70" s="7"/>
+      <c r="B70" s="8">
+        <v>0</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
+      <c r="A77" s="10"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="13"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
+      <c r="A87" s="10"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
+      <c r="A88" s="10"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
+      <c r="A89" s="10"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="13"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
+      <c r="A90" s="10"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="13"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
-      <c r="D91" s="13"/>
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="13"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="13"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="13"/>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="13"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="13"/>
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="13"/>
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="13"/>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="13"/>
+      <c r="A97" s="10"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="13"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
+      <c r="A98" s="10"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="13"/>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
+      <c r="A99" s="10"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="13"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
+      <c r="A100" s="10"/>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>